<commit_message>
Envío de fallos en el email a un .txt, empezando con el .log
</commit_message>
<xml_diff>
--- a/src/test/resources/testRight.xlsx
+++ b/src/test/resources/testRight.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6255"/>
+    <workbookView xWindow="5415" yWindow="3285" windowWidth="15030" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,7 +390,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Esquema completo de interfaces de la aplicación, algunas factorizaciones y posibilidad de generar salida de cartas en distintos formatos
</commit_message>
<xml_diff>
--- a/src/test/resources/testRight.xlsx
+++ b/src/test/resources/testRight.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nauce/Documents/censuses_2b/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="3285" windowWidth="15030" windowHeight="3690"/>
+    <workbookView xWindow="5420" yWindow="3280" windowWidth="15040" windowHeight="8180"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,15 +41,9 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>Ignacio Fernández Fernández</t>
-  </si>
-  <si>
     <t>56378435A</t>
   </si>
   <si>
-    <t>Naucé López González</t>
-  </si>
-  <si>
     <t>53678541Z</t>
   </si>
   <si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>jorge@uniovi.es</t>
+  </si>
+  <si>
+    <t>Ignacio Fernandez Fernandez</t>
+  </si>
+  <si>
+    <t>Nauce Lopez Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -379,7 +386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,16 +397,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,43 +420,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>220</v>

</xml_diff>

<commit_message>
Revert "Esquema completo de interfaces de la aplicación, algunas factorizaciones y posibilidad de generar salida de cartas en distintos formatos"
This reverts commit 239485ff7db8e3fc424f41f7e0b8626470d89001.
</commit_message>
<xml_diff>
--- a/src/test/resources/testRight.xlsx
+++ b/src/test/resources/testRight.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nauce/Documents/censuses_2b/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="3280" windowWidth="15040" windowHeight="8180"/>
+    <workbookView xWindow="5415" yWindow="3285" windowWidth="15030" windowHeight="3690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,9 +34,15 @@
     <t>Colegio</t>
   </si>
   <si>
+    <t>Ignacio Fernández Fernández</t>
+  </si>
+  <si>
     <t>56378435A</t>
   </si>
   <si>
+    <t>Naucé López González</t>
+  </si>
+  <si>
     <t>53678541Z</t>
   </si>
   <si>
@@ -60,12 +59,6 @@
   </si>
   <si>
     <t>jorge@uniovi.es</t>
-  </si>
-  <si>
-    <t>Ignacio Fernandez Fernandez</t>
-  </si>
-  <si>
-    <t>Nauce Lopez Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -386,7 +379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,16 +390,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,43 +413,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>220</v>

</xml_diff>

<commit_message>
Revert "Revert "Esquema completo de interfaces de la aplicación, algunas factorizaciones y posibilidad de generar salida de cartas en distintos formatos""
This reverts commit 2977f414384163db05a3329722ff26435c13764f.
</commit_message>
<xml_diff>
--- a/src/test/resources/testRight.xlsx
+++ b/src/test/resources/testRight.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nauce/Documents/censuses_2b/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="3285" windowWidth="15030" windowHeight="3690"/>
+    <workbookView xWindow="5420" yWindow="3280" windowWidth="15040" windowHeight="8180"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -34,15 +41,9 @@
     <t>Colegio</t>
   </si>
   <si>
-    <t>Ignacio Fernández Fernández</t>
-  </si>
-  <si>
     <t>56378435A</t>
   </si>
   <si>
-    <t>Naucé López González</t>
-  </si>
-  <si>
     <t>53678541Z</t>
   </si>
   <si>
@@ -59,6 +60,12 @@
   </si>
   <si>
     <t>jorge@uniovi.es</t>
+  </si>
+  <si>
+    <t>Ignacio Fernandez Fernandez</t>
+  </si>
+  <si>
+    <t>Nauce Lopez Gonzalez</t>
   </si>
 </sst>
 </file>
@@ -379,7 +386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -390,16 +397,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,43 +420,43 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>440</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4">
         <v>220</v>

</xml_diff>